<commit_message>
Update XLOOKUP Excel Tutorial File.xlsx
Only newer versions of excel have xlookup
</commit_message>
<xml_diff>
--- a/Excel/Lesson_22/XLOOKUP Excel Tutorial File.xlsx
+++ b/Excel/Lesson_22/XLOOKUP Excel Tutorial File.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\.vscode\Data_Analyst_Bootcamp\Excel\Lesson_22\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\.vscode\Data_Analyst_Bootcamp\Data_Analyst_Bootcamp\Excel\Lesson_22\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="XLookUp" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="XLookUp w SUM" sheetId="7" r:id="rId6"/>
     <sheet name="VLookUp" sheetId="2" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="93">
   <si>
     <t>EmployeeID</t>
   </si>
@@ -315,6 +315,9 @@
   </si>
   <si>
     <t>Address</t>
+  </si>
+  <si>
+    <t>Set to false, lookup value must be the first column of the table selected</t>
   </si>
 </sst>
 </file>
@@ -670,13 +673,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="40.7109375" bestFit="1" customWidth="1"/>
@@ -765,6 +769,10 @@
       <c r="A3" t="s">
         <v>65</v>
       </c>
+      <c r="B3" t="str">
+        <f>VLOOKUP(A3, $H$2:$P$10,9, FALSE)</f>
+        <v>Toby.Flenderson@DunderMifflinCorporate.com</v>
+      </c>
       <c r="E3">
         <v>1002</v>
       </c>
@@ -803,6 +811,10 @@
       <c r="A4" t="s">
         <v>62</v>
       </c>
+      <c r="B4" t="str">
+        <f t="shared" ref="B4:B6" si="0">VLOOKUP(A4, $H$2:$P$10,9, FALSE)</f>
+        <v>Pam.Beasley@DunderMifflin.com</v>
+      </c>
       <c r="E4">
         <v>1003</v>
       </c>
@@ -841,6 +853,10 @@
       <c r="A5" t="s">
         <v>67</v>
       </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>Meredith.Palmer@Yahoo.com</v>
+      </c>
       <c r="E5">
         <v>1004</v>
       </c>
@@ -879,6 +895,10 @@
       <c r="A6" t="s">
         <v>69</v>
       </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>Kevin.Malone@DunderMifflin.com</v>
+      </c>
       <c r="E6">
         <v>1005</v>
       </c>
@@ -1055,13 +1075,13 @@
     </row>
     <row r="22" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H22" t="str">
-        <f t="shared" ref="H22:H23" si="0">CONCATENATE(F12," ",G12)</f>
+        <f t="shared" ref="H22:H23" si="1">CONCATENATE(F12," ",G12)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="23" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -2668,18 +2688,20 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="44.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
         <v>0</v>
       </c>
@@ -2699,25 +2721,22 @@
         <v>4</v>
       </c>
       <c r="K1" t="s">
-        <v>91</v>
+        <v>5</v>
       </c>
       <c r="L1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -2742,26 +2761,30 @@
       <c r="J2" t="s">
         <v>12</v>
       </c>
-      <c r="L2" t="s">
+      <c r="K2" t="s">
         <v>13</v>
       </c>
-      <c r="M2">
+      <c r="L2">
         <v>45000</v>
       </c>
+      <c r="M2" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="N2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>63</v>
       </c>
+      <c r="B3" t="str">
+        <f>VLOOKUP(A3, H2:O10,8, FALSE)</f>
+        <v>Dwight.Schrute@AOL.com</v>
+      </c>
       <c r="E3">
         <v>1002</v>
       </c>
@@ -2780,26 +2803,30 @@
       <c r="J3" t="s">
         <v>19</v>
       </c>
-      <c r="L3" t="s">
+      <c r="K3" t="s">
         <v>20</v>
       </c>
-      <c r="M3">
+      <c r="L3">
         <v>36000</v>
       </c>
+      <c r="M3" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="N3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>66</v>
       </c>
+      <c r="B4" t="str">
+        <f t="shared" ref="B4:B5" si="0">VLOOKUP(A4, H3:O11,8, FALSE)</f>
+        <v>Michael.Scott@DunderMifflin.com</v>
+      </c>
       <c r="E4">
         <v>1003</v>
       </c>
@@ -2818,26 +2845,30 @@
       <c r="J4" t="s">
         <v>12</v>
       </c>
-      <c r="L4" t="s">
+      <c r="K4" t="s">
         <v>13</v>
       </c>
-      <c r="M4">
+      <c r="L4">
         <v>63000</v>
       </c>
+      <c r="M4" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="N4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>68</v>
       </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>Stanley.Hudson@gmail.com</v>
+      </c>
       <c r="E5">
         <v>1004</v>
       </c>
@@ -2856,23 +2887,23 @@
       <c r="J5" t="s">
         <v>19</v>
       </c>
-      <c r="L5" t="s">
+      <c r="K5" t="s">
         <v>31</v>
       </c>
-      <c r="M5">
+      <c r="L5">
         <v>47000</v>
       </c>
+      <c r="M5" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="N5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="O5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E6">
         <v>1005</v>
       </c>
@@ -2891,23 +2922,23 @@
       <c r="J6" t="s">
         <v>12</v>
       </c>
-      <c r="L6" t="s">
+      <c r="K6" t="s">
         <v>37</v>
       </c>
-      <c r="M6">
+      <c r="L6">
         <v>50000</v>
       </c>
+      <c r="M6" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="N6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="O6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E7">
         <v>1006</v>
       </c>
@@ -2926,23 +2957,23 @@
       <c r="J7" t="s">
         <v>12</v>
       </c>
-      <c r="L7" t="s">
+      <c r="K7" t="s">
         <v>43</v>
       </c>
-      <c r="M7">
+      <c r="L7">
         <v>65000</v>
       </c>
+      <c r="M7" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="N7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="O7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E8">
         <v>1007</v>
       </c>
@@ -2961,23 +2992,23 @@
       <c r="J8" t="s">
         <v>19</v>
       </c>
-      <c r="L8" t="s">
+      <c r="K8" t="s">
         <v>48</v>
       </c>
-      <c r="M8">
+      <c r="L8">
         <v>41000</v>
       </c>
+      <c r="M8" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="N8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="O8" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E9">
         <v>1008</v>
       </c>
@@ -2996,23 +3027,23 @@
       <c r="J9" t="s">
         <v>12</v>
       </c>
-      <c r="L9" t="s">
+      <c r="K9" t="s">
         <v>13</v>
       </c>
-      <c r="M9">
+      <c r="L9">
         <v>48000</v>
       </c>
+      <c r="M9" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="N9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="O9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="P9" s="2" t="s">
+      <c r="O9" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E10">
         <v>1009</v>
       </c>
@@ -3031,20 +3062,25 @@
       <c r="J10" t="s">
         <v>12</v>
       </c>
-      <c r="L10" t="s">
+      <c r="K10" t="s">
         <v>31</v>
       </c>
-      <c r="M10">
+      <c r="L10">
         <v>42000</v>
       </c>
+      <c r="M10" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="N10" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="O10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="P10" s="2" t="s">
+      <c r="O10" s="2" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>